<commit_message>
playing with the scenarios
</commit_message>
<xml_diff>
--- a/inactivation_scenarios.xlsx
+++ b/inactivation_scenarios.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://wageningenur4-my.sharepoint.com/personal/georgios_pampoukis_wur_nl/Documents/PhD components/Deliverables/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://wageningenur4-my.sharepoint.com/personal/georgios_pampoukis_wur_nl/Documents/PhD components/3rd year/qmra_project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1023" documentId="8_{EE042F72-7752-4F3F-B423-04B395C0905B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2D6E218C-F026-4F29-AFC1-3C9EF8D6AE6E}"/>
+  <xr:revisionPtr revIDLastSave="1038" documentId="8_{EE042F72-7752-4F3F-B423-04B395C0905B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0B99A686-063D-4A62-BC51-65DA1E0D574D}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{068B2558-D028-447E-BBE2-4CDF970AAB4D}"/>
   </bookViews>
@@ -530,10 +530,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEECA479-5C12-4697-986C-4E65010F9F27}">
-  <dimension ref="A1:W18"/>
+  <dimension ref="A1:W16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -573,7 +573,7 @@
         <v>26</v>
       </c>
       <c r="E2">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="G2" t="s">
         <v>32</v>
@@ -585,7 +585,7 @@
         <v>30</v>
       </c>
       <c r="K2">
-        <v>600</v>
+        <v>550</v>
       </c>
       <c r="M2" t="s">
         <v>2</v>
@@ -649,7 +649,7 @@
         <v>27</v>
       </c>
       <c r="E4">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="G4" t="s">
         <v>25</v>
@@ -661,7 +661,7 @@
         <v>27</v>
       </c>
       <c r="K4">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="M4" t="s">
         <v>4</v>
@@ -708,25 +708,25 @@
       </c>
       <c r="B6">
         <f>B2+(B3-E2)/B4</f>
-        <v>-2.4842857142857144</v>
+        <v>-1.9485714285714286</v>
       </c>
       <c r="D6" t="s">
         <v>37</v>
       </c>
       <c r="E6">
         <f>E4*60</f>
-        <v>30</v>
+        <v>6</v>
       </c>
       <c r="G6" t="s">
         <v>33</v>
       </c>
       <c r="H6">
         <f>H2+(H3-K2)/H4</f>
-        <v>-0.6903703703703703</v>
+        <v>-0.50518518518518518</v>
       </c>
       <c r="K6">
         <f>60*K4</f>
-        <v>300</v>
+        <v>60</v>
       </c>
       <c r="M6" t="s">
         <v>11</v>
@@ -760,14 +760,14 @@
       </c>
       <c r="B7">
         <f>10^B6</f>
-        <v>3.278795162898284E-3</v>
+        <v>1.125715306862485E-2</v>
       </c>
       <c r="G7" t="s">
         <v>12</v>
       </c>
       <c r="H7">
         <f>10^H6</f>
-        <v>0.20399974738253523</v>
+        <v>0.31247466765083171</v>
       </c>
       <c r="M7" t="s">
         <v>12</v>
@@ -795,14 +795,14 @@
       </c>
       <c r="B8">
         <f>E4/B7</f>
-        <v>152.49504014701122</v>
+        <v>8.8832406728760773</v>
       </c>
       <c r="G8" t="s">
         <v>13</v>
       </c>
       <c r="H8">
         <f>K4/H7</f>
-        <v>24.509834272608803</v>
+        <v>3.2002594242853282</v>
       </c>
       <c r="M8" t="s">
         <v>13</v>
@@ -859,7 +859,7 @@
         <v>36</v>
       </c>
       <c r="E12">
-        <v>79.5</v>
+        <v>103</v>
       </c>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.25">
@@ -876,13 +876,7 @@
       </c>
       <c r="B16">
         <f>B12+E12/40</f>
-        <v>2.7175000000000002</v>
-      </c>
-    </row>
-    <row r="18" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D18">
-        <f>152/5</f>
-        <v>30.4</v>
+        <v>3.3050000000000002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>